<commit_message>
Refactor code to enhance type hints and improve filtering logic in pipeline service
</commit_message>
<xml_diff>
--- a/resultado_pipeline.xlsx
+++ b/resultado_pipeline.xlsx
@@ -3225,7 +3225,7 @@
         </is>
       </c>
       <c r="J74" t="n">
-        <v>431288.7399999999</v>
+        <v>431288.74</v>
       </c>
       <c r="K74" t="n">
         <v>21300</v>
@@ -10385,7 +10385,7 @@
       <c r="H254" t="inlineStr"/>
       <c r="I254" t="inlineStr"/>
       <c r="J254" t="n">
-        <v>50144.35999999999</v>
+        <v>50144.36</v>
       </c>
       <c r="K254" t="n">
         <v>0</v>
@@ -10681,7 +10681,7 @@
       <c r="H262" t="inlineStr"/>
       <c r="I262" t="inlineStr"/>
       <c r="J262" t="n">
-        <v>55425.49000000001</v>
+        <v>55425.49</v>
       </c>
       <c r="K262" t="n">
         <v>0</v>
@@ -11384,7 +11384,7 @@
       <c r="H281" t="inlineStr"/>
       <c r="I281" t="inlineStr"/>
       <c r="J281" t="n">
-        <v>935.4</v>
+        <v>935.4000000000001</v>
       </c>
       <c r="K281" t="n">
         <v>0</v>
@@ -13234,7 +13234,7 @@
       <c r="H331" t="inlineStr"/>
       <c r="I331" t="inlineStr"/>
       <c r="J331" t="n">
-        <v>71623.59999999998</v>
+        <v>71623.60000000002</v>
       </c>
       <c r="K331" t="n">
         <v>0</v>
@@ -14401,7 +14401,7 @@
       <c r="H362" t="inlineStr"/>
       <c r="I362" t="inlineStr"/>
       <c r="J362" t="n">
-        <v>638075.9400000001</v>
+        <v>638075.9400000002</v>
       </c>
       <c r="K362" t="n">
         <v>0</v>
@@ -14475,7 +14475,7 @@
       <c r="H364" t="inlineStr"/>
       <c r="I364" t="inlineStr"/>
       <c r="J364" t="n">
-        <v>514248.7799999999</v>
+        <v>514248.78</v>
       </c>
       <c r="K364" t="n">
         <v>0</v>
@@ -14549,7 +14549,7 @@
       <c r="H366" t="inlineStr"/>
       <c r="I366" t="inlineStr"/>
       <c r="J366" t="n">
-        <v>277910.4099999999</v>
+        <v>277910.41</v>
       </c>
       <c r="K366" t="n">
         <v>0</v>
@@ -16399,7 +16399,7 @@
       <c r="H416" t="inlineStr"/>
       <c r="I416" t="inlineStr"/>
       <c r="J416" t="n">
-        <v>75245.06999999999</v>
+        <v>75245.06999999998</v>
       </c>
       <c r="K416" t="n">
         <v>0</v>
@@ -19011,7 +19011,7 @@
       <c r="H482" t="inlineStr"/>
       <c r="I482" t="inlineStr"/>
       <c r="J482" t="n">
-        <v>109115.46</v>
+        <v>109115.4599999999</v>
       </c>
       <c r="K482" t="n">
         <v>0</v>
@@ -19418,7 +19418,7 @@
       <c r="H493" t="inlineStr"/>
       <c r="I493" t="inlineStr"/>
       <c r="J493" t="n">
-        <v>92214.14999999999</v>
+        <v>92214.15000000001</v>
       </c>
       <c r="K493" t="n">
         <v>0</v>
@@ -29101,7 +29101,7 @@
       <c r="H754" t="inlineStr"/>
       <c r="I754" t="inlineStr"/>
       <c r="J754" t="n">
-        <v>9966.99</v>
+        <v>9966.990000000002</v>
       </c>
       <c r="K754" t="n">
         <v>0</v>
@@ -29249,7 +29249,7 @@
       <c r="H758" t="inlineStr"/>
       <c r="I758" t="inlineStr"/>
       <c r="J758" t="n">
-        <v>7940.400000000001</v>
+        <v>7940.4</v>
       </c>
       <c r="K758" t="n">
         <v>0</v>
@@ -30137,7 +30137,7 @@
       <c r="H782" t="inlineStr"/>
       <c r="I782" t="inlineStr"/>
       <c r="J782" t="n">
-        <v>67520.37000000001</v>
+        <v>67520.37</v>
       </c>
       <c r="K782" t="n">
         <v>0</v>
@@ -30332,7 +30332,7 @@
         </is>
       </c>
       <c r="J787" t="n">
-        <v>417522.64</v>
+        <v>417522.6400000001</v>
       </c>
       <c r="K787" t="n">
         <v>8910656</v>
@@ -30426,7 +30426,7 @@
         </is>
       </c>
       <c r="J789" t="n">
-        <v>354606.9799999999</v>
+        <v>354606.98</v>
       </c>
       <c r="K789" t="n">
         <v>0</v>
@@ -30520,7 +30520,7 @@
         </is>
       </c>
       <c r="J791" t="n">
-        <v>385426.47</v>
+        <v>385426.4699999999</v>
       </c>
       <c r="K791" t="n">
         <v>0</v>
@@ -30708,7 +30708,7 @@
         </is>
       </c>
       <c r="J795" t="n">
-        <v>391701.6599999998</v>
+        <v>391701.6599999999</v>
       </c>
       <c r="K795" t="n">
         <v>0</v>
@@ -30755,7 +30755,7 @@
         </is>
       </c>
       <c r="J796" t="n">
-        <v>452400.9599999998</v>
+        <v>452400.96</v>
       </c>
       <c r="K796" t="n">
         <v>0</v>
@@ -30802,7 +30802,7 @@
         </is>
       </c>
       <c r="J797" t="n">
-        <v>292577.5699999999</v>
+        <v>292577.5700000001</v>
       </c>
       <c r="K797" t="n">
         <v>0</v>
@@ -30849,7 +30849,7 @@
         </is>
       </c>
       <c r="J798" t="n">
-        <v>565817.7699999998</v>
+        <v>565817.77</v>
       </c>
       <c r="K798" t="n">
         <v>0</v>
@@ -30896,7 +30896,7 @@
         </is>
       </c>
       <c r="J799" t="n">
-        <v>539673.5700000001</v>
+        <v>539673.5699999999</v>
       </c>
       <c r="K799" t="n">
         <v>0</v>
@@ -30943,7 +30943,7 @@
         </is>
       </c>
       <c r="J800" t="n">
-        <v>538262.0599999999</v>
+        <v>538262.0600000001</v>
       </c>
       <c r="K800" t="n">
         <v>0</v>
@@ -30990,7 +30990,7 @@
         </is>
       </c>
       <c r="J801" t="n">
-        <v>460942.19</v>
+        <v>460942.1899999999</v>
       </c>
       <c r="K801" t="n">
         <v>0</v>
@@ -31037,7 +31037,7 @@
         </is>
       </c>
       <c r="J802" t="n">
-        <v>484541.1599999998</v>
+        <v>484541.1599999999</v>
       </c>
       <c r="K802" t="n">
         <v>0</v>
@@ -31131,7 +31131,7 @@
         </is>
       </c>
       <c r="J804" t="n">
-        <v>495349.36</v>
+        <v>495349.3600000002</v>
       </c>
       <c r="K804" t="n">
         <v>0</v>
@@ -31178,7 +31178,7 @@
         </is>
       </c>
       <c r="J805" t="n">
-        <v>356352.1300000001</v>
+        <v>356352.13</v>
       </c>
       <c r="K805" t="n">
         <v>0</v>
@@ -31225,7 +31225,7 @@
         </is>
       </c>
       <c r="J806" t="n">
-        <v>536627.51</v>
+        <v>536627.5099999998</v>
       </c>
       <c r="K806" t="n">
         <v>0</v>
@@ -31319,7 +31319,7 @@
         </is>
       </c>
       <c r="J808" t="n">
-        <v>407207.1899999999</v>
+        <v>407207.1900000001</v>
       </c>
       <c r="K808" t="n">
         <v>0</v>
@@ -31366,7 +31366,7 @@
         </is>
       </c>
       <c r="J809" t="n">
-        <v>408936.9300000001</v>
+        <v>408936.93</v>
       </c>
       <c r="K809" t="n">
         <v>0</v>
@@ -31460,7 +31460,7 @@
         </is>
       </c>
       <c r="J811" t="n">
-        <v>506029.5799999998</v>
+        <v>506029.58</v>
       </c>
       <c r="K811" t="n">
         <v>0</v>
@@ -31507,7 +31507,7 @@
         </is>
       </c>
       <c r="J812" t="n">
-        <v>304013.3700000001</v>
+        <v>304013.37</v>
       </c>
       <c r="K812" t="n">
         <v>0</v>
@@ -31601,7 +31601,7 @@
         </is>
       </c>
       <c r="J814" t="n">
-        <v>365435.64</v>
+        <v>365435.6400000001</v>
       </c>
       <c r="K814" t="n">
         <v>0</v>
@@ -31695,7 +31695,7 @@
         </is>
       </c>
       <c r="J816" t="n">
-        <v>554254.97</v>
+        <v>554254.9700000001</v>
       </c>
       <c r="K816" t="n">
         <v>0</v>
@@ -31789,7 +31789,7 @@
         </is>
       </c>
       <c r="J818" t="n">
-        <v>398440.5299999999</v>
+        <v>398440.53</v>
       </c>
       <c r="K818" t="n">
         <v>0</v>
@@ -31836,7 +31836,7 @@
         </is>
       </c>
       <c r="J819" t="n">
-        <v>531192.0900000001</v>
+        <v>531192.09</v>
       </c>
       <c r="K819" t="n">
         <v>0</v>
@@ -31883,7 +31883,7 @@
         </is>
       </c>
       <c r="J820" t="n">
-        <v>474333.0099999998</v>
+        <v>474333.01</v>
       </c>
       <c r="K820" t="n">
         <v>0</v>
@@ -31930,7 +31930,7 @@
         </is>
       </c>
       <c r="J821" t="n">
-        <v>331450.04</v>
+        <v>331450.0400000001</v>
       </c>
       <c r="K821" t="n">
         <v>0</v>
@@ -31977,7 +31977,7 @@
         </is>
       </c>
       <c r="J822" t="n">
-        <v>288810.44</v>
+        <v>288810.4399999999</v>
       </c>
       <c r="K822" t="n">
         <v>0</v>
@@ -32118,7 +32118,7 @@
         </is>
       </c>
       <c r="J825" t="n">
-        <v>578475.0000000003</v>
+        <v>578475.0000000001</v>
       </c>
       <c r="K825" t="n">
         <v>0</v>
@@ -32165,7 +32165,7 @@
         </is>
       </c>
       <c r="J826" t="n">
-        <v>604554.1299999998</v>
+        <v>604554.13</v>
       </c>
       <c r="K826" t="n">
         <v>0</v>
@@ -32212,7 +32212,7 @@
         </is>
       </c>
       <c r="J827" t="n">
-        <v>491313.5199999999</v>
+        <v>491313.52</v>
       </c>
       <c r="K827" t="n">
         <v>0</v>
@@ -32259,7 +32259,7 @@
         </is>
       </c>
       <c r="J828" t="n">
-        <v>516983.3100000002</v>
+        <v>516983.3099999998</v>
       </c>
       <c r="K828" t="n">
         <v>0</v>
@@ -32306,7 +32306,7 @@
         </is>
       </c>
       <c r="J829" t="n">
-        <v>649116.0399999997</v>
+        <v>649116.0399999998</v>
       </c>
       <c r="K829" t="n">
         <v>0</v>
@@ -32353,7 +32353,7 @@
         </is>
       </c>
       <c r="J830" t="n">
-        <v>440629.0799999998</v>
+        <v>440629.08</v>
       </c>
       <c r="K830" t="n">
         <v>0</v>
@@ -32400,7 +32400,7 @@
         </is>
       </c>
       <c r="J831" t="n">
-        <v>460517.5</v>
+        <v>460517.5000000001</v>
       </c>
       <c r="K831" t="n">
         <v>0</v>
@@ -32447,7 +32447,7 @@
         </is>
       </c>
       <c r="J832" t="n">
-        <v>373838.0499999998</v>
+        <v>373838.05</v>
       </c>
       <c r="K832" t="n">
         <v>0</v>
@@ -32494,7 +32494,7 @@
         </is>
       </c>
       <c r="J833" t="n">
-        <v>493637.2199999998</v>
+        <v>493637.22</v>
       </c>
       <c r="K833" t="n">
         <v>0</v>
@@ -32588,7 +32588,7 @@
         </is>
       </c>
       <c r="J835" t="n">
-        <v>338129.3999999998</v>
+        <v>338129.4</v>
       </c>
       <c r="K835" t="n">
         <v>0</v>
@@ -33062,7 +33062,7 @@
         </is>
       </c>
       <c r="J847" t="n">
-        <v>799968.4400000001</v>
+        <v>799968.4399999999</v>
       </c>
       <c r="K847" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Enhance logging level to DEBUG and add detailed logs in the pipeline service for better traceability
</commit_message>
<xml_diff>
--- a/resultado_pipeline.xlsx
+++ b/resultado_pipeline.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sebraesp-my.sharepoint.com/personal/cesargl_sebraesp_com_br/Documents/Área de Trabalho/receitas_orc/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_C145083E0BBFE78A383294F63BAD32FF7879A039" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{769880C4-5035-4488-8056-FC0CBB752C01}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Resultado" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -73,7 +67,7 @@
     <t>Aprop_Mes_Empresas_Beneficiadas</t>
   </si>
   <si>
-    <t>ACUMULADO_DESPESA</t>
+    <t>ACUMULADO</t>
   </si>
   <si>
     <t>Total_Apropriado_Acumulado</t>
@@ -790,8 +784,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -845,8 +843,8 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -856,21 +854,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -908,7 +898,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -942,7 +932,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -977,10 +966,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1153,26 +1141,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="6" max="9" width="18.7109375" style="1" customWidth="1"/>
     <col min="10" max="12" width="12.7109375" style="2" customWidth="1"/>
-    <col min="13" max="16" width="18.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.7109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="48.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="18.7109375" style="1" customWidth="1"/>
+    <col min="13" max="22" width="18.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1240,7 +1221,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1308,7 +1289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1376,7 +1357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1444,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1497,13 +1478,13 @@
         <v>0</v>
       </c>
       <c r="R5" s="1">
-        <v>1267860.1000000001</v>
+        <v>1267860.1</v>
       </c>
       <c r="S5" s="1">
-        <v>1267860.1000000001</v>
+        <v>1267860.1</v>
       </c>
       <c r="T5" s="1">
-        <v>1267860.1000000001</v>
+        <v>1267860.1</v>
       </c>
       <c r="U5" s="1">
         <v>0</v>
@@ -1512,7 +1493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1580,7 +1561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1648,7 +1629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1716,7 +1697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1784,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1813,13 +1794,13 @@
         <v>18000</v>
       </c>
       <c r="J10" s="2">
-        <v>0.38793103448275862</v>
+        <v>0.3879310344827586</v>
       </c>
       <c r="K10" s="2">
-        <v>0.53448275862068961</v>
+        <v>0.5344827586206896</v>
       </c>
       <c r="L10" s="2">
-        <v>7.7586206896551727E-2</v>
+        <v>0.07758620689655173</v>
       </c>
       <c r="M10" s="1">
         <v>0</v>
@@ -1852,7 +1833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1920,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1952,10 +1933,10 @@
         <v>0.4999986710362993</v>
       </c>
       <c r="K12" s="2">
-        <v>0.30000026579274008</v>
+        <v>0.3000002657927401</v>
       </c>
       <c r="L12" s="2">
-        <v>0.20000106317096061</v>
+        <v>0.2000010631709606</v>
       </c>
       <c r="M12" s="1">
         <v>17160</v>
@@ -1964,13 +1945,13 @@
         <v>17160</v>
       </c>
       <c r="O12" s="1">
-        <v>8579.9771949828955</v>
+        <v>8579.977194982896</v>
       </c>
       <c r="P12" s="1">
-        <v>5148.0045610034203</v>
+        <v>5148.00456100342</v>
       </c>
       <c r="Q12" s="1">
-        <v>3432.0182440136832</v>
+        <v>3432.018244013683</v>
       </c>
       <c r="R12" s="1">
         <v>18506.14</v>
@@ -1982,13 +1963,13 @@
         <v>9253.045406011699</v>
       </c>
       <c r="U12" s="1">
-        <v>5551.8469187976598</v>
+        <v>5551.84691879766</v>
       </c>
       <c r="V12" s="1">
-        <v>3701.2476751906402</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+        <v>3701.24767519064</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2032,13 +2013,13 @@
         <v>488</v>
       </c>
       <c r="O13" s="1">
-        <v>243.99935146571411</v>
+        <v>243.9993514657141</v>
       </c>
       <c r="P13" s="1">
         <v>146.4001297068572</v>
       </c>
       <c r="Q13" s="1">
-        <v>97.600518827428758</v>
+        <v>97.60051882742876</v>
       </c>
       <c r="R13" s="1">
         <v>8288</v>
@@ -2047,16 +2028,16 @@
         <v>8288</v>
       </c>
       <c r="T13" s="1">
-        <v>4143.9889855488482</v>
+        <v>4143.988985548848</v>
       </c>
       <c r="U13" s="1">
         <v>2486.40220289023</v>
       </c>
       <c r="V13" s="1">
-        <v>1657.6088115609209</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+        <v>1657.608811560921</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -2124,7 +2105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2153,13 +2134,13 @@
         <v>28043</v>
       </c>
       <c r="J15" s="2">
-        <v>0.33330003472569081</v>
+        <v>0.3333000347256908</v>
       </c>
       <c r="K15" s="2">
-        <v>0.60000047569439485</v>
+        <v>0.6000004756943949</v>
       </c>
       <c r="L15" s="2">
-        <v>6.6699489579914284E-2</v>
+        <v>0.06669948957991428</v>
       </c>
       <c r="M15" s="1">
         <v>20087.8</v>
@@ -2168,22 +2149,22 @@
         <v>20087.8</v>
       </c>
       <c r="O15" s="1">
-        <v>6695.2644375627306</v>
+        <v>6695.264437562731</v>
       </c>
       <c r="P15" s="1">
         <v>12052.68955565386</v>
       </c>
       <c r="Q15" s="1">
-        <v>1339.8460067834019</v>
+        <v>1339.846006783402</v>
       </c>
       <c r="R15" s="1">
         <v>40703.4</v>
       </c>
       <c r="S15" s="1">
-        <v>40703.399999999987</v>
+        <v>40703.39999999999</v>
       </c>
       <c r="T15" s="1">
-        <v>13566.444633453681</v>
+        <v>13566.44463345368</v>
       </c>
       <c r="U15" s="1">
         <v>24422.05936237923</v>
@@ -2192,7 +2173,7 @@
         <v>2714.896004167083</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2251,16 +2232,16 @@
         <v>12573.9</v>
       </c>
       <c r="T16" s="1">
-        <v>4190.8813066373632</v>
+        <v>4190.881306637363</v>
       </c>
       <c r="U16" s="1">
-        <v>7544.3459813337513</v>
+        <v>7544.345981333751</v>
       </c>
       <c r="V16" s="1">
-        <v>838.67271202888423</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+        <v>838.6727120288842</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2307,10 +2288,10 @@
         <v>236.2430646135696</v>
       </c>
       <c r="P17" s="1">
-        <v>425.28033717218699</v>
+        <v>425.280337172187</v>
       </c>
       <c r="Q17" s="1">
-        <v>47.276598214243243</v>
+        <v>47.27659821424324</v>
       </c>
       <c r="R17" s="1">
         <v>25664.99</v>
@@ -2319,7 +2300,7 @@
         <v>25664.99</v>
       </c>
       <c r="T17" s="1">
-        <v>8554.1420582345072</v>
+        <v>8554.142058234507</v>
       </c>
       <c r="U17" s="1">
         <v>15399.00620869189</v>
@@ -2328,7 +2309,7 @@
         <v>1711.841733073604</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2396,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2464,7 +2445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -2532,7 +2513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -2561,10 +2542,10 @@
         <v>0</v>
       </c>
       <c r="J21" s="2">
-        <v>0.61324999999999996</v>
+        <v>0.61325</v>
       </c>
       <c r="K21" s="2">
-        <v>0.38674999999999998</v>
+        <v>0.38675</v>
       </c>
       <c r="L21" s="2">
         <v>0</v>
@@ -2591,16 +2572,16 @@
         <v>64425.2</v>
       </c>
       <c r="T21" s="1">
-        <v>39508.753900000003</v>
+        <v>39508.7539</v>
       </c>
       <c r="U21" s="1">
-        <v>24916.446100000001</v>
+        <v>24916.4461</v>
       </c>
       <c r="V21" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -2659,7 +2640,7 @@
         <v>7200</v>
       </c>
       <c r="T22" s="1">
-        <v>4415.3999999999996</v>
+        <v>4415.4</v>
       </c>
       <c r="U22" s="1">
         <v>2784.6</v>
@@ -2668,7 +2649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -2697,13 +2678,13 @@
         <v>121000</v>
       </c>
       <c r="J23" s="2">
-        <v>0.20607994724353351</v>
+        <v>0.2060799472435335</v>
       </c>
       <c r="K23" s="2">
-        <v>0.70486407555479669</v>
+        <v>0.7048640755547967</v>
       </c>
       <c r="L23" s="2">
-        <v>8.9055977201669842E-2</v>
+        <v>0.08905597720166984</v>
       </c>
       <c r="M23" s="1">
         <v>15708</v>
@@ -2712,7 +2693,7 @@
         <v>15708</v>
       </c>
       <c r="O23" s="1">
-        <v>3237.1038113014238</v>
+        <v>3237.103811301424</v>
       </c>
       <c r="P23" s="1">
         <v>11072.00489881475</v>
@@ -2727,16 +2708,16 @@
         <v>90588</v>
       </c>
       <c r="T23" s="1">
-        <v>18668.370260897209</v>
+        <v>18668.37026089721</v>
       </c>
       <c r="U23" s="1">
         <v>63852.22687635792</v>
       </c>
       <c r="V23" s="1">
-        <v>8067.4028627448679</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+        <v>8067.402862744868</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -2792,19 +2773,19 @@
         <v>838.8</v>
       </c>
       <c r="S24" s="1">
-        <v>838.80000000000007</v>
+        <v>838.8000000000001</v>
       </c>
       <c r="T24" s="1">
         <v>172.8598597478759</v>
       </c>
       <c r="U24" s="1">
-        <v>591.23998657536345</v>
+        <v>591.2399865753634</v>
       </c>
       <c r="V24" s="1">
-        <v>74.700153676760664</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+        <v>74.70015367676066</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -2872,7 +2853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -2940,7 +2921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -2978,7 +2959,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="1">
-        <v>1233.8499999999999</v>
+        <v>1233.85</v>
       </c>
       <c r="N27" s="1">
         <v>0</v>
@@ -2993,7 +2974,7 @@
         <v>0</v>
       </c>
       <c r="R27" s="1">
-        <v>1233.8499999999999</v>
+        <v>1233.85</v>
       </c>
       <c r="S27" s="1">
         <v>0</v>
@@ -3008,7 +2989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -3046,7 +3027,7 @@
         <v>0</v>
       </c>
       <c r="M28" s="1">
-        <v>10146.719999999999</v>
+        <v>10146.72</v>
       </c>
       <c r="N28" s="1">
         <v>0</v>
@@ -3076,7 +3057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -3144,7 +3125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -3212,7 +3193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -3280,7 +3261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -3348,7 +3329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -3416,7 +3397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -3454,10 +3435,10 @@
         <v>1</v>
       </c>
       <c r="M34" s="1">
-        <v>1100.8800000000051</v>
+        <v>1100.880000000005</v>
       </c>
       <c r="N34" s="1">
-        <v>1100.8800000000051</v>
+        <v>1100.880000000005</v>
       </c>
       <c r="O34" s="1">
         <v>0</v>
@@ -3466,7 +3447,7 @@
         <v>0</v>
       </c>
       <c r="Q34" s="1">
-        <v>1100.8800000000051</v>
+        <v>1100.880000000005</v>
       </c>
       <c r="R34" s="1">
         <v>12053.38</v>
@@ -3484,7 +3465,7 @@
         <v>12053.38</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -3552,7 +3533,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -3620,7 +3601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -3688,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -3756,7 +3737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -3824,7 +3805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -3892,7 +3873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22">
       <c r="A41" t="s">
         <v>37</v>
       </c>
@@ -3960,7 +3941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -4028,7 +4009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -4096,7 +4077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -4164,7 +4145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -4232,7 +4213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22">
       <c r="A46" t="s">
         <v>37</v>
       </c>
@@ -4300,7 +4281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -4368,7 +4349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -4436,7 +4417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22">
       <c r="A49" t="s">
         <v>37</v>
       </c>
@@ -4504,7 +4485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -4557,22 +4538,22 @@
         <v>0</v>
       </c>
       <c r="R50" s="1">
-        <v>22443.919999999998</v>
+        <v>22443.92</v>
       </c>
       <c r="S50" s="1">
-        <v>22443.919999999998</v>
+        <v>22443.92</v>
       </c>
       <c r="T50" s="1">
         <v>0</v>
       </c>
       <c r="U50" s="1">
-        <v>22443.919999999998</v>
+        <v>22443.92</v>
       </c>
       <c r="V50" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22">
       <c r="A51" t="s">
         <v>37</v>
       </c>
@@ -4640,7 +4621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -4708,7 +4689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22">
       <c r="A53" t="s">
         <v>37</v>
       </c>
@@ -4746,16 +4727,16 @@
         <v>0</v>
       </c>
       <c r="M53" s="1">
-        <v>78271.290000000008</v>
+        <v>78271.29000000001</v>
       </c>
       <c r="N53" s="1">
-        <v>78271.290000000008</v>
+        <v>78271.29000000001</v>
       </c>
       <c r="O53" s="1">
         <v>0</v>
       </c>
       <c r="P53" s="1">
-        <v>78271.290000000008</v>
+        <v>78271.29000000001</v>
       </c>
       <c r="Q53" s="1">
         <v>0</v>
@@ -4776,7 +4757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22">
       <c r="A54" t="s">
         <v>38</v>
       </c>
@@ -4844,7 +4825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22">
       <c r="A55" t="s">
         <v>38</v>
       </c>
@@ -4912,7 +4893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22">
       <c r="A56" t="s">
         <v>38</v>
       </c>
@@ -4980,7 +4961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22">
       <c r="A57" t="s">
         <v>39</v>
       </c>
@@ -5048,7 +5029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22">
       <c r="A58" t="s">
         <v>39</v>
       </c>
@@ -5101,13 +5082,13 @@
         <v>0</v>
       </c>
       <c r="R58" s="1">
-        <v>5522164.3499999996</v>
+        <v>5522164.35</v>
       </c>
       <c r="S58" s="1">
-        <v>5522164.3499999996</v>
+        <v>5522164.35</v>
       </c>
       <c r="T58" s="1">
-        <v>5522164.3499999996</v>
+        <v>5522164.35</v>
       </c>
       <c r="U58" s="1">
         <v>0</v>
@@ -5116,7 +5097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22">
       <c r="A59" t="s">
         <v>39</v>
       </c>
@@ -5184,7 +5165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -5252,7 +5233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22">
       <c r="A61" t="s">
         <v>39</v>
       </c>
@@ -5290,13 +5271,13 @@
         <v>0</v>
       </c>
       <c r="M61" s="1">
-        <v>385426.47000000009</v>
+        <v>385426.4700000001</v>
       </c>
       <c r="N61" s="1">
-        <v>385426.47000000009</v>
+        <v>385426.4700000001</v>
       </c>
       <c r="O61" s="1">
-        <v>385426.47000000009</v>
+        <v>385426.4700000001</v>
       </c>
       <c r="P61" s="1">
         <v>0</v>
@@ -5320,7 +5301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22">
       <c r="A62" t="s">
         <v>39</v>
       </c>
@@ -5358,13 +5339,13 @@
         <v>0</v>
       </c>
       <c r="M62" s="1">
-        <v>320673.21000000008</v>
+        <v>320673.2100000001</v>
       </c>
       <c r="N62" s="1">
-        <v>320673.21000000008</v>
+        <v>320673.2100000001</v>
       </c>
       <c r="O62" s="1">
-        <v>320673.21000000008</v>
+        <v>320673.2100000001</v>
       </c>
       <c r="P62" s="1">
         <v>0</v>
@@ -5388,7 +5369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22">
       <c r="A63" t="s">
         <v>39</v>
       </c>
@@ -5426,13 +5407,13 @@
         <v>0</v>
       </c>
       <c r="M63" s="1">
-        <v>406655.55999999988</v>
+        <v>406655.5599999999</v>
       </c>
       <c r="N63" s="1">
-        <v>406655.55999999988</v>
+        <v>406655.5599999999</v>
       </c>
       <c r="O63" s="1">
-        <v>406655.55999999988</v>
+        <v>406655.5599999999</v>
       </c>
       <c r="P63" s="1">
         <v>0</v>
@@ -5456,7 +5437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22">
       <c r="A64" t="s">
         <v>39</v>
       </c>
@@ -5524,7 +5505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22">
       <c r="A65" t="s">
         <v>39</v>
       </c>
@@ -5562,13 +5543,13 @@
         <v>0</v>
       </c>
       <c r="M65" s="1">
-        <v>391701.65999999992</v>
+        <v>391701.6599999999</v>
       </c>
       <c r="N65" s="1">
-        <v>391701.65999999992</v>
+        <v>391701.6599999999</v>
       </c>
       <c r="O65" s="1">
-        <v>391701.65999999992</v>
+        <v>391701.6599999999</v>
       </c>
       <c r="P65" s="1">
         <v>0</v>
@@ -5592,7 +5573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22">
       <c r="A66" t="s">
         <v>39</v>
       </c>
@@ -5660,7 +5641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22">
       <c r="A67" t="s">
         <v>39</v>
       </c>
@@ -5698,13 +5679,13 @@
         <v>0</v>
       </c>
       <c r="M67" s="1">
-        <v>292577.56999999989</v>
+        <v>292577.5699999999</v>
       </c>
       <c r="N67" s="1">
-        <v>292577.56999999989</v>
+        <v>292577.5699999999</v>
       </c>
       <c r="O67" s="1">
-        <v>292577.56999999989</v>
+        <v>292577.5699999999</v>
       </c>
       <c r="P67" s="1">
         <v>0</v>
@@ -5728,7 +5709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22">
       <c r="A68" t="s">
         <v>39</v>
       </c>
@@ -5796,7 +5777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22">
       <c r="A69" t="s">
         <v>39</v>
       </c>
@@ -5834,13 +5815,13 @@
         <v>0</v>
       </c>
       <c r="M69" s="1">
-        <v>539673.56999999995</v>
+        <v>539673.5699999999</v>
       </c>
       <c r="N69" s="1">
-        <v>539673.56999999995</v>
+        <v>539673.5699999999</v>
       </c>
       <c r="O69" s="1">
-        <v>539673.56999999995</v>
+        <v>539673.5699999999</v>
       </c>
       <c r="P69" s="1">
         <v>0</v>
@@ -5849,13 +5830,13 @@
         <v>0</v>
       </c>
       <c r="R69" s="1">
-        <v>2605408.4900000002</v>
+        <v>2605408.49</v>
       </c>
       <c r="S69" s="1">
-        <v>2605408.4900000002</v>
+        <v>2605408.49</v>
       </c>
       <c r="T69" s="1">
-        <v>2605408.4900000002</v>
+        <v>2605408.49</v>
       </c>
       <c r="U69" s="1">
         <v>0</v>
@@ -5864,7 +5845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22">
       <c r="A70" t="s">
         <v>39</v>
       </c>
@@ -5902,13 +5883,13 @@
         <v>0</v>
       </c>
       <c r="M70" s="1">
-        <v>538262.06000000006</v>
+        <v>538262.0600000001</v>
       </c>
       <c r="N70" s="1">
-        <v>538262.06000000006</v>
+        <v>538262.0600000001</v>
       </c>
       <c r="O70" s="1">
-        <v>538262.06000000006</v>
+        <v>538262.0600000001</v>
       </c>
       <c r="P70" s="1">
         <v>0</v>
@@ -5917,13 +5898,13 @@
         <v>0</v>
       </c>
       <c r="R70" s="1">
-        <v>2625975.0299999998</v>
+        <v>2625975.03</v>
       </c>
       <c r="S70" s="1">
-        <v>2625975.0299999998</v>
+        <v>2625975.03</v>
       </c>
       <c r="T70" s="1">
-        <v>2625975.0299999998</v>
+        <v>2625975.03</v>
       </c>
       <c r="U70" s="1">
         <v>0</v>
@@ -5932,7 +5913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22">
       <c r="A71" t="s">
         <v>39</v>
       </c>
@@ -5985,13 +5966,13 @@
         <v>0</v>
       </c>
       <c r="R71" s="1">
-        <v>2381271.7799999998</v>
+        <v>2381271.78</v>
       </c>
       <c r="S71" s="1">
-        <v>2381271.7799999998</v>
+        <v>2381271.78</v>
       </c>
       <c r="T71" s="1">
-        <v>2381271.7799999998</v>
+        <v>2381271.78</v>
       </c>
       <c r="U71" s="1">
         <v>0</v>
@@ -6000,7 +5981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -6068,7 +6049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22">
       <c r="A73" t="s">
         <v>39</v>
       </c>
@@ -6106,13 +6087,13 @@
         <v>0</v>
       </c>
       <c r="M73" s="1">
-        <v>438242.51000000018</v>
+        <v>438242.5100000002</v>
       </c>
       <c r="N73" s="1">
-        <v>438242.51000000018</v>
+        <v>438242.5100000002</v>
       </c>
       <c r="O73" s="1">
-        <v>438242.51000000018</v>
+        <v>438242.5100000002</v>
       </c>
       <c r="P73" s="1">
         <v>0</v>
@@ -6136,7 +6117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22">
       <c r="A74" t="s">
         <v>39</v>
       </c>
@@ -6204,7 +6185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22">
       <c r="A75" t="s">
         <v>39</v>
       </c>
@@ -6242,13 +6223,13 @@
         <v>0</v>
       </c>
       <c r="M75" s="1">
-        <v>356352.12999999989</v>
+        <v>356352.1299999999</v>
       </c>
       <c r="N75" s="1">
-        <v>356352.12999999989</v>
+        <v>356352.1299999999</v>
       </c>
       <c r="O75" s="1">
-        <v>356352.12999999989</v>
+        <v>356352.1299999999</v>
       </c>
       <c r="P75" s="1">
         <v>0</v>
@@ -6272,7 +6253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22">
       <c r="A76" t="s">
         <v>39</v>
       </c>
@@ -6310,13 +6291,13 @@
         <v>0</v>
       </c>
       <c r="M76" s="1">
-        <v>536627.50999999989</v>
+        <v>536627.5099999999</v>
       </c>
       <c r="N76" s="1">
-        <v>536627.50999999989</v>
+        <v>536627.5099999999</v>
       </c>
       <c r="O76" s="1">
-        <v>536627.50999999989</v>
+        <v>536627.5099999999</v>
       </c>
       <c r="P76" s="1">
         <v>0</v>
@@ -6340,7 +6321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22">
       <c r="A77" t="s">
         <v>39</v>
       </c>
@@ -6378,13 +6359,13 @@
         <v>0</v>
       </c>
       <c r="M77" s="1">
-        <v>365110.47999999992</v>
+        <v>365110.4799999999</v>
       </c>
       <c r="N77" s="1">
-        <v>365110.47999999992</v>
+        <v>365110.4799999999</v>
       </c>
       <c r="O77" s="1">
-        <v>365110.47999999992</v>
+        <v>365110.4799999999</v>
       </c>
       <c r="P77" s="1">
         <v>0</v>
@@ -6408,7 +6389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22">
       <c r="A78" t="s">
         <v>39</v>
       </c>
@@ -6446,13 +6427,13 @@
         <v>0</v>
       </c>
       <c r="M78" s="1">
-        <v>407207.18999999989</v>
+        <v>407207.1899999999</v>
       </c>
       <c r="N78" s="1">
-        <v>407207.18999999989</v>
+        <v>407207.1899999999</v>
       </c>
       <c r="O78" s="1">
-        <v>407207.18999999989</v>
+        <v>407207.1899999999</v>
       </c>
       <c r="P78" s="1">
         <v>0</v>
@@ -6476,7 +6457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22">
       <c r="A79" t="s">
         <v>39</v>
       </c>
@@ -6514,13 +6495,13 @@
         <v>0</v>
       </c>
       <c r="M79" s="1">
-        <v>408936.92999999988</v>
+        <v>408936.9299999999</v>
       </c>
       <c r="N79" s="1">
-        <v>408936.92999999988</v>
+        <v>408936.9299999999</v>
       </c>
       <c r="O79" s="1">
-        <v>408936.92999999988</v>
+        <v>408936.9299999999</v>
       </c>
       <c r="P79" s="1">
         <v>0</v>
@@ -6544,7 +6525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22">
       <c r="A80" t="s">
         <v>39</v>
       </c>
@@ -6612,7 +6593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:22">
       <c r="A81" t="s">
         <v>39</v>
       </c>
@@ -6650,13 +6631,13 @@
         <v>0</v>
       </c>
       <c r="M81" s="1">
-        <v>506029.58000000007</v>
+        <v>506029.5800000001</v>
       </c>
       <c r="N81" s="1">
-        <v>506029.58000000007</v>
+        <v>506029.5800000001</v>
       </c>
       <c r="O81" s="1">
-        <v>506029.58000000007</v>
+        <v>506029.5800000001</v>
       </c>
       <c r="P81" s="1">
         <v>0</v>
@@ -6680,7 +6661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:22">
       <c r="A82" t="s">
         <v>39</v>
       </c>
@@ -6748,7 +6729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:22">
       <c r="A83" t="s">
         <v>39</v>
       </c>
@@ -6801,13 +6782,13 @@
         <v>0</v>
       </c>
       <c r="R83" s="1">
-        <v>2164286.7999999998</v>
+        <v>2164286.8</v>
       </c>
       <c r="S83" s="1">
-        <v>2164286.7999999998</v>
+        <v>2164286.8</v>
       </c>
       <c r="T83" s="1">
-        <v>2164286.7999999998</v>
+        <v>2164286.8</v>
       </c>
       <c r="U83" s="1">
         <v>0</v>
@@ -6816,7 +6797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:22">
       <c r="A84" t="s">
         <v>39</v>
       </c>
@@ -6884,7 +6865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:22">
       <c r="A85" t="s">
         <v>39</v>
       </c>
@@ -6937,13 +6918,13 @@
         <v>0</v>
       </c>
       <c r="R85" s="1">
-        <v>2342772.0699999998</v>
+        <v>2342772.07</v>
       </c>
       <c r="S85" s="1">
-        <v>2342772.0699999998</v>
+        <v>2342772.07</v>
       </c>
       <c r="T85" s="1">
-        <v>2342772.0699999998</v>
+        <v>2342772.07</v>
       </c>
       <c r="U85" s="1">
         <v>0</v>
@@ -6952,7 +6933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:22">
       <c r="A86" t="s">
         <v>39</v>
       </c>
@@ -7020,7 +7001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:22">
       <c r="A87" t="s">
         <v>39</v>
       </c>
@@ -7058,13 +7039,13 @@
         <v>0</v>
       </c>
       <c r="M87" s="1">
-        <v>277696.78999999998</v>
+        <v>277696.79</v>
       </c>
       <c r="N87" s="1">
-        <v>277696.78999999998</v>
+        <v>277696.79</v>
       </c>
       <c r="O87" s="1">
-        <v>277696.78999999998</v>
+        <v>277696.79</v>
       </c>
       <c r="P87" s="1">
         <v>0</v>
@@ -7088,7 +7069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:22">
       <c r="A88" t="s">
         <v>39</v>
       </c>
@@ -7156,7 +7137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:22">
       <c r="A89" t="s">
         <v>39</v>
       </c>
@@ -7209,13 +7190,13 @@
         <v>0</v>
       </c>
       <c r="R89" s="1">
-        <v>2584725.0499999998</v>
+        <v>2584725.05</v>
       </c>
       <c r="S89" s="1">
-        <v>2584725.0499999998</v>
+        <v>2584725.05</v>
       </c>
       <c r="T89" s="1">
-        <v>2584725.0499999998</v>
+        <v>2584725.05</v>
       </c>
       <c r="U89" s="1">
         <v>0</v>
@@ -7224,7 +7205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:22">
       <c r="A90" t="s">
         <v>39</v>
       </c>
@@ -7292,7 +7273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:22">
       <c r="A91" t="s">
         <v>39</v>
       </c>
@@ -7330,13 +7311,13 @@
         <v>0</v>
       </c>
       <c r="M91" s="1">
-        <v>331450.03999999998</v>
+        <v>331450.04</v>
       </c>
       <c r="N91" s="1">
-        <v>331450.03999999998</v>
+        <v>331450.04</v>
       </c>
       <c r="O91" s="1">
-        <v>331450.03999999998</v>
+        <v>331450.04</v>
       </c>
       <c r="P91" s="1">
         <v>0</v>
@@ -7360,7 +7341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:22">
       <c r="A92" t="s">
         <v>39</v>
       </c>
@@ -7398,13 +7379,13 @@
         <v>0</v>
       </c>
       <c r="M92" s="1">
-        <v>288810.43999999989</v>
+        <v>288810.4399999999</v>
       </c>
       <c r="N92" s="1">
-        <v>288810.43999999989</v>
+        <v>288810.4399999999</v>
       </c>
       <c r="O92" s="1">
-        <v>288810.43999999989</v>
+        <v>288810.4399999999</v>
       </c>
       <c r="P92" s="1">
         <v>0</v>
@@ -7428,7 +7409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:22">
       <c r="A93" t="s">
         <v>39</v>
       </c>
@@ -7466,13 +7447,13 @@
         <v>0</v>
       </c>
       <c r="M93" s="1">
-        <v>321363.15000000002</v>
+        <v>321363.15</v>
       </c>
       <c r="N93" s="1">
-        <v>321363.15000000002</v>
+        <v>321363.15</v>
       </c>
       <c r="O93" s="1">
-        <v>321363.15000000002</v>
+        <v>321363.15</v>
       </c>
       <c r="P93" s="1">
         <v>0</v>
@@ -7496,7 +7477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:22">
       <c r="A94" t="s">
         <v>39</v>
       </c>
@@ -7564,7 +7545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:22">
       <c r="A95" t="s">
         <v>39</v>
       </c>
@@ -7602,13 +7583,13 @@
         <v>0</v>
       </c>
       <c r="M95" s="1">
-        <v>578475.00000000023</v>
+        <v>578475.0000000002</v>
       </c>
       <c r="N95" s="1">
-        <v>578475.00000000023</v>
+        <v>578475.0000000002</v>
       </c>
       <c r="O95" s="1">
-        <v>578475.00000000023</v>
+        <v>578475.0000000002</v>
       </c>
       <c r="P95" s="1">
         <v>0</v>
@@ -7617,13 +7598,13 @@
         <v>0</v>
       </c>
       <c r="R95" s="1">
-        <v>2835870.0500000012</v>
+        <v>2835870.050000001</v>
       </c>
       <c r="S95" s="1">
-        <v>2835870.0500000012</v>
+        <v>2835870.050000001</v>
       </c>
       <c r="T95" s="1">
-        <v>2835870.0500000012</v>
+        <v>2835870.050000001</v>
       </c>
       <c r="U95" s="1">
         <v>0</v>
@@ -7632,7 +7613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:22">
       <c r="A96" t="s">
         <v>39</v>
       </c>
@@ -7700,7 +7681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22">
       <c r="A97" t="s">
         <v>39</v>
       </c>
@@ -7768,7 +7749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22">
       <c r="A98" t="s">
         <v>39</v>
       </c>
@@ -7806,13 +7787,13 @@
         <v>0</v>
       </c>
       <c r="M98" s="1">
-        <v>516983.31000000011</v>
+        <v>516983.3100000001</v>
       </c>
       <c r="N98" s="1">
-        <v>516983.31000000011</v>
+        <v>516983.3100000001</v>
       </c>
       <c r="O98" s="1">
-        <v>516983.31000000011</v>
+        <v>516983.3100000001</v>
       </c>
       <c r="P98" s="1">
         <v>0</v>
@@ -7836,7 +7817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22">
       <c r="A99" t="s">
         <v>39</v>
       </c>
@@ -7904,7 +7885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22">
       <c r="A100" t="s">
         <v>39</v>
       </c>
@@ -7957,13 +7938,13 @@
         <v>0</v>
       </c>
       <c r="R100" s="1">
-        <v>2529109.9300000002</v>
+        <v>2529109.93</v>
       </c>
       <c r="S100" s="1">
-        <v>2529109.9300000002</v>
+        <v>2529109.93</v>
       </c>
       <c r="T100" s="1">
-        <v>2529109.9300000002</v>
+        <v>2529109.93</v>
       </c>
       <c r="U100" s="1">
         <v>0</v>
@@ -7972,7 +7953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22">
       <c r="A101" t="s">
         <v>39</v>
       </c>
@@ -8010,13 +7991,13 @@
         <v>0</v>
       </c>
       <c r="M101" s="1">
-        <v>460517.50000000012</v>
+        <v>460517.5000000001</v>
       </c>
       <c r="N101" s="1">
-        <v>460517.50000000012</v>
+        <v>460517.5000000001</v>
       </c>
       <c r="O101" s="1">
-        <v>460517.50000000012</v>
+        <v>460517.5000000001</v>
       </c>
       <c r="P101" s="1">
         <v>0</v>
@@ -8025,13 +8006,13 @@
         <v>0</v>
       </c>
       <c r="R101" s="1">
-        <v>2190929.5699999998</v>
+        <v>2190929.57</v>
       </c>
       <c r="S101" s="1">
-        <v>2190929.5699999998</v>
+        <v>2190929.57</v>
       </c>
       <c r="T101" s="1">
-        <v>2190929.5699999998</v>
+        <v>2190929.57</v>
       </c>
       <c r="U101" s="1">
         <v>0</v>
@@ -8040,7 +8021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22">
       <c r="A102" t="s">
         <v>39</v>
       </c>
@@ -8108,7 +8089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:22">
       <c r="A103" t="s">
         <v>39</v>
       </c>
@@ -8161,13 +8142,13 @@
         <v>0</v>
       </c>
       <c r="R103" s="1">
-        <v>2358485.7799999998</v>
+        <v>2358485.78</v>
       </c>
       <c r="S103" s="1">
-        <v>2358485.7799999998</v>
+        <v>2358485.78</v>
       </c>
       <c r="T103" s="1">
-        <v>2358485.7799999998</v>
+        <v>2358485.78</v>
       </c>
       <c r="U103" s="1">
         <v>0</v>
@@ -8176,7 +8157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22">
       <c r="A104" t="s">
         <v>39</v>
       </c>
@@ -8244,7 +8225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22">
       <c r="A105" t="s">
         <v>39</v>
       </c>
@@ -8282,13 +8263,13 @@
         <v>0</v>
       </c>
       <c r="M105" s="1">
-        <v>338129.40000000008</v>
+        <v>338129.4000000001</v>
       </c>
       <c r="N105" s="1">
-        <v>338129.40000000008</v>
+        <v>338129.4000000001</v>
       </c>
       <c r="O105" s="1">
-        <v>338129.40000000008</v>
+        <v>338129.4000000001</v>
       </c>
       <c r="P105" s="1">
         <v>0</v>
@@ -8312,7 +8293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:22">
       <c r="A106" t="s">
         <v>40</v>
       </c>
@@ -8380,7 +8361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:22">
       <c r="A107" t="s">
         <v>40</v>
       </c>
@@ -8448,7 +8429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:22">
       <c r="A108" t="s">
         <v>40</v>
       </c>
@@ -8486,13 +8467,13 @@
         <v>0</v>
       </c>
       <c r="M108" s="1">
-        <v>799968.44000000006</v>
+        <v>799968.4400000001</v>
       </c>
       <c r="N108" s="1">
-        <v>799968.44000000006</v>
+        <v>799968.4400000001</v>
       </c>
       <c r="O108" s="1">
-        <v>799968.44000000006</v>
+        <v>799968.4400000001</v>
       </c>
       <c r="P108" s="1">
         <v>0</v>
@@ -8501,13 +8482,13 @@
         <v>0</v>
       </c>
       <c r="R108" s="1">
-        <v>8441501.4399999995</v>
+        <v>8441501.439999999</v>
       </c>
       <c r="S108" s="1">
-        <v>8441501.4399999995</v>
+        <v>8441501.439999999</v>
       </c>
       <c r="T108" s="1">
-        <v>8441501.4399999995</v>
+        <v>8441501.439999999</v>
       </c>
       <c r="U108" s="1">
         <v>0</v>
@@ -8516,7 +8497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:22">
       <c r="A109" t="s">
         <v>40</v>
       </c>
@@ -8586,14 +8567,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;K0000FF Classificação: RESTRITA&amp;1#_x000D_</oddHeader>
-  </headerFooter>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{549d7762-508d-44f8-a2ae-91da522b0310}" enabled="1" method="Standard" siteId="{6d60b55c-2576-4d60-ae33-11df0ea07983}" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>